<commit_message>
Built site for MassWateR: 1.0.0.9000@0545e2b
</commit_message>
<xml_diff>
--- a/ExampleResults.xlsx
+++ b/ExampleResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA845B59-DFA3-44BD-B103-00ACC15942F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B333CB1-DF5A-459C-A543-F9D9326D0E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="30885" yWindow="1095" windowWidth="23595" windowHeight="13380" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16083" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16086" uniqueCount="142">
   <si>
     <t>Monitoring Location ID</t>
   </si>
@@ -496,6 +496,15 @@
   <si>
     <t>pH-6-17-5</t>
   </si>
+  <si>
+    <t>Sample Collection Method ID</t>
+  </si>
+  <si>
+    <t>Project ID</t>
+  </si>
+  <si>
+    <t>Result Comment</t>
+  </si>
 </sst>
 </file>
 
@@ -578,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,6 +610,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -918,13 +930,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N2653"/>
+  <dimension ref="A1:Q2653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E957" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I968" sqref="I968"/>
+      <selection pane="bottomRight" activeCell="N963" sqref="N963"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,9 +951,12 @@
     <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -984,8 +999,17 @@
       <c r="N1" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +1041,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1049,7 +1073,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1081,7 +1105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1113,7 +1137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1145,7 +1169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1177,7 +1201,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1241,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1305,7 +1329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1337,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1401,7 +1425,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1433,7 +1457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Built site for MassWateR: 1.0.0.9000@3820c2d
</commit_message>
<xml_diff>
--- a/ExampleResults.xlsx
+++ b/ExampleResults.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B333CB1-DF5A-459C-A543-F9D9326D0E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FD2931-E460-4182-A1AF-B481EDFDFE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="1095" windowWidth="23595" windowHeight="13380" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
+    <workbookView xWindow="2355" yWindow="915" windowWidth="21600" windowHeight="11325" xr2:uid="{6EB090EE-BC59-4E27-A120-D58B60EE5B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$N$2500</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$1:$Q$2653</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -383,9 +383,6 @@
     <t>cfu/100ml</t>
   </si>
   <si>
-    <t>Quality Control Field Calibration Check</t>
-  </si>
-  <si>
     <t>K16452-MB1</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   <si>
     <t>Result Comment</t>
   </si>
+  <si>
+    <t>Quality Control-Calibration Check</t>
+  </si>
 </sst>
 </file>
 
@@ -587,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -610,9 +610,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -933,10 +930,10 @@
   <dimension ref="A1:Q2653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E957" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2620" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N963" sqref="N963"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,14 +996,14 @@
       <c r="N1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -82579,7 +82576,7 @@
         <v>96</v>
       </c>
       <c r="N2545" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2546" spans="2:14" x14ac:dyDescent="0.25">
@@ -82599,7 +82596,7 @@
         <v>96</v>
       </c>
       <c r="N2546" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2547" spans="2:14" x14ac:dyDescent="0.25">
@@ -82619,7 +82616,7 @@
         <v>96</v>
       </c>
       <c r="N2547" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2548" spans="2:14" x14ac:dyDescent="0.25">
@@ -82639,7 +82636,7 @@
         <v>96</v>
       </c>
       <c r="N2548" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2549" spans="2:14" x14ac:dyDescent="0.25">
@@ -82659,7 +82656,7 @@
         <v>96</v>
       </c>
       <c r="N2549" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2550" spans="2:14" x14ac:dyDescent="0.25">
@@ -82679,7 +82676,7 @@
         <v>96</v>
       </c>
       <c r="N2550" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2551" spans="2:14" x14ac:dyDescent="0.25">
@@ -82699,7 +82696,7 @@
         <v>96</v>
       </c>
       <c r="N2551" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2552" spans="2:14" x14ac:dyDescent="0.25">
@@ -82719,7 +82716,7 @@
         <v>96</v>
       </c>
       <c r="N2552" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2553" spans="2:14" x14ac:dyDescent="0.25">
@@ -82833,7 +82830,7 @@
         <v>13</v>
       </c>
       <c r="N2558" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2559" spans="2:14" x14ac:dyDescent="0.25">
@@ -82859,7 +82856,7 @@
         <v>13</v>
       </c>
       <c r="N2559" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2560" spans="2:14" x14ac:dyDescent="0.25">
@@ -82885,7 +82882,7 @@
         <v>13</v>
       </c>
       <c r="N2560" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2561" spans="2:14" x14ac:dyDescent="0.25">
@@ -82911,7 +82908,7 @@
         <v>13</v>
       </c>
       <c r="N2561" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2562" spans="2:14" x14ac:dyDescent="0.25">
@@ -82937,7 +82934,7 @@
         <v>13</v>
       </c>
       <c r="N2562" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2563" spans="2:14" x14ac:dyDescent="0.25">
@@ -82963,7 +82960,7 @@
         <v>13</v>
       </c>
       <c r="N2563" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2564" spans="2:14" x14ac:dyDescent="0.25">
@@ -82992,7 +82989,7 @@
         <v>13</v>
       </c>
       <c r="N2564" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2565" spans="2:14" x14ac:dyDescent="0.25">
@@ -83021,7 +83018,7 @@
         <v>13</v>
       </c>
       <c r="N2565" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2566" spans="2:14" x14ac:dyDescent="0.25">
@@ -83050,7 +83047,7 @@
         <v>13</v>
       </c>
       <c r="N2566" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2567" spans="2:14" x14ac:dyDescent="0.25">
@@ -83079,7 +83076,7 @@
         <v>13</v>
       </c>
       <c r="N2567" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2568" spans="2:14" x14ac:dyDescent="0.25">
@@ -83108,7 +83105,7 @@
         <v>13</v>
       </c>
       <c r="N2568" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2569" spans="2:14" x14ac:dyDescent="0.25">
@@ -83137,7 +83134,7 @@
         <v>13</v>
       </c>
       <c r="N2569" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2570" spans="2:14" x14ac:dyDescent="0.25">
@@ -83166,7 +83163,7 @@
         <v>13</v>
       </c>
       <c r="N2570" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2571" spans="2:14" x14ac:dyDescent="0.25">
@@ -83195,7 +83192,7 @@
         <v>13</v>
       </c>
       <c r="N2571" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2572" spans="2:14" x14ac:dyDescent="0.25">
@@ -83224,7 +83221,7 @@
         <v>13</v>
       </c>
       <c r="N2572" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2573" spans="2:14" x14ac:dyDescent="0.25">
@@ -83256,7 +83253,7 @@
         <v>13</v>
       </c>
       <c r="N2573" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2574" spans="2:14" x14ac:dyDescent="0.25">
@@ -83288,7 +83285,7 @@
         <v>13</v>
       </c>
       <c r="N2574" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2575" spans="2:14" x14ac:dyDescent="0.25">
@@ -83713,7 +83710,7 @@
         <v>13</v>
       </c>
       <c r="N2593" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2594" spans="2:14" x14ac:dyDescent="0.25">
@@ -83742,7 +83739,7 @@
         <v>13</v>
       </c>
       <c r="N2594" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2595" spans="2:14" x14ac:dyDescent="0.25">
@@ -83771,7 +83768,7 @@
         <v>13</v>
       </c>
       <c r="N2595" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2596" spans="2:14" x14ac:dyDescent="0.25">
@@ -83800,7 +83797,7 @@
         <v>13</v>
       </c>
       <c r="N2596" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2597" spans="2:14" x14ac:dyDescent="0.25">
@@ -83829,7 +83826,7 @@
         <v>13</v>
       </c>
       <c r="N2597" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2598" spans="2:14" x14ac:dyDescent="0.25">
@@ -83858,7 +83855,7 @@
         <v>13</v>
       </c>
       <c r="N2598" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2599" spans="2:14" x14ac:dyDescent="0.25">
@@ -84443,7 +84440,7 @@
     </row>
     <row r="2628" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2628" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2628" s="4">
         <v>44360</v>
@@ -84467,12 +84464,12 @@
         <v>13</v>
       </c>
       <c r="N2628" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2629" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2629" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2629" s="4">
         <v>44360</v>
@@ -84496,12 +84493,12 @@
         <v>13</v>
       </c>
       <c r="N2629" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2630" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2630" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2630" s="4">
         <v>44360</v>
@@ -84525,12 +84522,12 @@
         <v>13</v>
       </c>
       <c r="N2630" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2631" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2631" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2631" s="4">
         <v>44360</v>
@@ -84554,12 +84551,12 @@
         <v>13</v>
       </c>
       <c r="N2631" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2632" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2632" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2632" s="4">
         <v>44362</v>
@@ -84583,12 +84580,12 @@
         <v>13</v>
       </c>
       <c r="N2632" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2633" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2633" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2633" s="4">
         <v>44363</v>
@@ -84612,12 +84609,12 @@
         <v>13</v>
       </c>
       <c r="N2633" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2634" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2634" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2634" s="4">
         <v>44364</v>
@@ -84641,12 +84638,12 @@
         <v>13</v>
       </c>
       <c r="N2634" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2635" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2635" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2635" s="4">
         <v>44360</v>
@@ -84670,12 +84667,12 @@
         <v>13</v>
       </c>
       <c r="N2635" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2636" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2636" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2636" s="4">
         <v>44360</v>
@@ -84699,12 +84696,12 @@
         <v>13</v>
       </c>
       <c r="N2636" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2637" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2637" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2637" s="4">
         <v>44451</v>
@@ -84730,7 +84727,7 @@
     </row>
     <row r="2638" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2638" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2638" s="4">
         <v>44451</v>
@@ -84756,7 +84753,7 @@
     </row>
     <row r="2639" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2639" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2639" s="4">
         <v>44451</v>
@@ -84782,7 +84779,7 @@
     </row>
     <row r="2640" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2640" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2640" s="4">
         <v>44451</v>
@@ -84808,7 +84805,7 @@
     </row>
     <row r="2641" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2641" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2641" s="4">
         <v>44451</v>
@@ -84834,7 +84831,7 @@
     </row>
     <row r="2642" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2642" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2642" s="4">
         <v>44451</v>
@@ -84860,7 +84857,7 @@
     </row>
     <row r="2643" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2643" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2643" s="4">
         <v>44451</v>
@@ -84886,7 +84883,7 @@
     </row>
     <row r="2644" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2644" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2644" s="4">
         <v>44420</v>
@@ -84912,7 +84909,7 @@
     </row>
     <row r="2645" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2645" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2645" s="4">
         <v>44451</v>
@@ -84938,7 +84935,7 @@
     </row>
     <row r="2646" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2646" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2646" s="4">
         <v>44451</v>
@@ -84964,7 +84961,7 @@
     </row>
     <row r="2647" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2647" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2647" s="4">
         <v>44451</v>
@@ -84990,7 +84987,7 @@
     </row>
     <row r="2648" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2648" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2648" s="4">
         <v>44481</v>
@@ -85016,7 +85013,7 @@
     </row>
     <row r="2649" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2649" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2649" s="4">
         <v>44482</v>
@@ -85042,7 +85039,7 @@
     </row>
     <row r="2650" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2650" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2650" s="4">
         <v>44483</v>
@@ -85068,7 +85065,7 @@
     </row>
     <row r="2651" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2651" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2651" s="4">
         <v>44484</v>
@@ -85094,7 +85091,7 @@
     </row>
     <row r="2652" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2652" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2652" s="4">
         <v>44484</v>
@@ -85120,7 +85117,7 @@
     </row>
     <row r="2653" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2653" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="C2653" s="4">
         <v>44485</v>
@@ -85145,6 +85142,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q2653" xr:uid="{C271A468-9B9D-48BE-A50F-E841236CDECF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N2649">
     <sortCondition ref="B2:B2649"/>
     <sortCondition ref="H2:H2649"/>

</xml_diff>